<commit_message>
modified:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/.ipynb_checkpoints/NaT_Model_Development-checkpoint.ipynb 	modified:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/NaT_Model_Development.ipynb 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/Sim_10.dat 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/figure_12.jpeg 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/figure_13.jpeg 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/figure_14.jpeg 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/figure_15.jpeg 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/figure_16.jpeg 	modified:   AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/iAMC_kinetics.xlsx
</commit_message>
<xml_diff>
--- a/AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/iAMC_kinetics.xlsx
+++ b/AccessoryOlfactoryBulb/MitralCell/ipython/NaT_MultipleChannelModel/iAMC_kinetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
   <si>
     <t>SD</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>Vmembrane</t>
+  </si>
+  <si>
+    <t>G_Gmax_mean</t>
   </si>
 </sst>
 </file>
@@ -69,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -86,6 +92,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,13 +1115,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Q4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="4">
@@ -1322,6 +1332,218 @@
         <v>0</v>
       </c>
       <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>-100</v>
+      </c>
+      <c r="C6">
+        <v>-90</v>
+      </c>
+      <c r="D6">
+        <v>-80</v>
+      </c>
+      <c r="E6">
+        <v>-70</v>
+      </c>
+      <c r="F6">
+        <v>-60</v>
+      </c>
+      <c r="G6">
+        <v>-50</v>
+      </c>
+      <c r="H6">
+        <v>-40</v>
+      </c>
+      <c r="I6">
+        <v>-30</v>
+      </c>
+      <c r="J6">
+        <v>-20</v>
+      </c>
+      <c r="K6">
+        <v>-10</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+      <c r="O6">
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.93</v>
+      </c>
+      <c r="C7">
+        <v>0.89</v>
+      </c>
+      <c r="D7">
+        <v>0.98</v>
+      </c>
+      <c r="E7">
+        <v>0.99</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.82273458300000002</v>
+      </c>
+      <c r="H7">
+        <v>0.460393948</v>
+      </c>
+      <c r="I7">
+        <v>0.22382597400000001</v>
+      </c>
+      <c r="J7">
+        <v>0.114555137</v>
+      </c>
+      <c r="K7">
+        <v>5.8905299000000001E-2</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>2.8169200000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>1.5103699999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>9.0817299999999997E-3</v>
+      </c>
+      <c r="F8">
+        <v>2.9301600000000001E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.118613</v>
+      </c>
+      <c r="H8">
+        <v>0.159719</v>
+      </c>
+      <c r="I8">
+        <v>0.127634</v>
+      </c>
+      <c r="J8">
+        <v>8.6147000000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>6.5250699999999995E-2</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1.9918599999999998E-3</v>
+      </c>
+      <c r="D9">
+        <v>1.068E-2</v>
+      </c>
+      <c r="E9">
+        <v>6.4217500000000004E-3</v>
+      </c>
+      <c r="F9">
+        <v>9.7672100000000001E-3</v>
+      </c>
+      <c r="G9">
+        <v>3.9537599999999999E-2</v>
+      </c>
+      <c r="H9">
+        <v>5.3239700000000001E-2</v>
+      </c>
+      <c r="I9">
+        <v>4.2544600000000002E-2</v>
+      </c>
+      <c r="J9">
+        <v>2.87157E-2</v>
+      </c>
+      <c r="K9">
+        <v>2.1750200000000001E-2</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>0</v>
       </c>
     </row>
@@ -1332,13 +1554,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="4">
@@ -1549,6 +1774,218 @@
         <v>5.8558699999999998E-2</v>
       </c>
     </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>-100</v>
+      </c>
+      <c r="C6">
+        <v>-90</v>
+      </c>
+      <c r="D6">
+        <v>-80</v>
+      </c>
+      <c r="E6">
+        <v>-70</v>
+      </c>
+      <c r="F6">
+        <v>-60</v>
+      </c>
+      <c r="G6">
+        <v>-50</v>
+      </c>
+      <c r="H6">
+        <v>-40</v>
+      </c>
+      <c r="I6">
+        <v>-30</v>
+      </c>
+      <c r="J6">
+        <v>-20</v>
+      </c>
+      <c r="K6">
+        <v>-10</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+      <c r="O6">
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.15113407200000001</v>
+      </c>
+      <c r="H7">
+        <v>0.65212565199999994</v>
+      </c>
+      <c r="I7">
+        <v>0.71021805199999999</v>
+      </c>
+      <c r="J7">
+        <v>0.72966279199999995</v>
+      </c>
+      <c r="K7">
+        <v>0.75403364799999995</v>
+      </c>
+      <c r="L7">
+        <v>0.78516262400000003</v>
+      </c>
+      <c r="M7">
+        <v>0.80887361199999996</v>
+      </c>
+      <c r="N7">
+        <v>0.84201415899999998</v>
+      </c>
+      <c r="O7">
+        <v>0.88799295899999997</v>
+      </c>
+      <c r="P7">
+        <v>0.94068791100000004</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.43665900000000002</v>
+      </c>
+      <c r="H8">
+        <v>1.7643499999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>3.0018699999999999E-2</v>
+      </c>
+      <c r="J8">
+        <v>3.8357200000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>5.5595499999999999E-2</v>
+      </c>
+      <c r="L8">
+        <v>6.7766300000000002E-2</v>
+      </c>
+      <c r="M8">
+        <v>8.6252300000000004E-2</v>
+      </c>
+      <c r="N8">
+        <v>0.107416</v>
+      </c>
+      <c r="O8">
+        <v>0.12745500000000001</v>
+      </c>
+      <c r="P8">
+        <v>0.15342500000000001</v>
+      </c>
+      <c r="Q8">
+        <v>0.175676</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0.14555299999999999</v>
+      </c>
+      <c r="H9">
+        <v>5.8811699999999998E-3</v>
+      </c>
+      <c r="I9">
+        <v>1.00062E-2</v>
+      </c>
+      <c r="J9">
+        <v>1.2785700000000001E-2</v>
+      </c>
+      <c r="K9">
+        <v>1.8531800000000001E-2</v>
+      </c>
+      <c r="L9">
+        <v>2.2588799999999999E-2</v>
+      </c>
+      <c r="M9">
+        <v>2.87508E-2</v>
+      </c>
+      <c r="N9">
+        <v>3.5805299999999998E-2</v>
+      </c>
+      <c r="O9">
+        <v>4.2484899999999999E-2</v>
+      </c>
+      <c r="P9">
+        <v>5.1141499999999999E-2</v>
+      </c>
+      <c r="Q9">
+        <v>5.8558699999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>